<commit_message>
Add correlation copula in thmodel_simple example
</commit_message>
<xml_diff>
--- a/model_TH_macos/inputs/default_th_values1.xlsx
+++ b/model_TH_macos/inputs/default_th_values1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaperin_macos/Documents/PhD/3_Academic/Code/Julia/BN/model_TH_macos/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E000FF-3667-354A-8CDF-3ADE5D8FB260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F9EACC-EE10-C04D-9235-8501BE2A0062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{1040DAD3-1126-084A-BFBA-50ECC4DEFFE6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>gamma</t>
   </si>
@@ -117,16 +117,10 @@
     <t>K_y</t>
   </si>
   <si>
-    <t>K_z</t>
-  </si>
-  <si>
     <t>Kx</t>
   </si>
   <si>
     <t>Ky</t>
-  </si>
-  <si>
-    <t>Kz</t>
   </si>
   <si>
     <t>disp_longh</t>
@@ -488,8 +482,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{56CBCCD3-825D-FC43-BB43-C16A41D0AE3B}" name="Table2" displayName="Table2" ref="A1:D38" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D38" xr:uid="{56CBCCD3-825D-FC43-BB43-C16A41D0AE3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{56CBCCD3-825D-FC43-BB43-C16A41D0AE3B}" name="Table2" displayName="Table2" ref="A1:D37" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D37" xr:uid="{56CBCCD3-825D-FC43-BB43-C16A41D0AE3B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B43907B2-BD59-A543-A64F-6EED5E99A285}" name="name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{408DEB97-0FDA-8145-AF54-E2DA6C85B28A}" name="value" dataDxfId="2"/>
@@ -866,30 +860,30 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5">
         <v>190</v>
@@ -898,7 +892,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="7">
         <v>210</v>
@@ -907,7 +901,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" s="5">
         <v>25</v>
@@ -916,7 +910,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="7">
         <v>50</v>
@@ -925,35 +919,35 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="7">
         <v>0.08</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5">
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="7">
         <v>5.9999999999999997E-7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -963,10 +957,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FC343A-6120-C049-B7A4-2C3A911D4D0B}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1078,7 +1072,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1087,12 +1081,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1101,12 +1095,12 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -1115,12 +1109,12 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1129,12 +1123,12 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
         <v>400</v>
@@ -1143,12 +1137,12 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1157,12 +1151,12 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1">
         <v>50</v>
@@ -1171,12 +1165,12 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1">
         <v>200</v>
@@ -1185,12 +1179,12 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1199,12 +1193,12 @@
         <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>25</v>
@@ -1213,12 +1207,12 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1227,12 +1221,12 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -1241,12 +1235,12 @@
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <f>B15*B16*B17</f>
@@ -1256,12 +1250,12 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1">
         <f>B15+1</f>
@@ -1271,12 +1265,12 @@
         <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1">
         <f>B15+1</f>
@@ -1286,40 +1280,40 @@
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1">
         <v>0.2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1">
         <f>0*10*(-5)</f>
@@ -1329,12 +1323,12 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1">
         <f>B15/2-25+1</f>
@@ -1344,12 +1338,12 @@
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1">
         <f>B15/2+25+1</f>
@@ -1359,26 +1353,26 @@
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
@@ -1387,12 +1381,12 @@
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
@@ -1401,12 +1395,12 @@
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -1415,12 +1409,12 @@
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -1429,7 +1423,7 @@
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1441,15 +1435,15 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1">
         <f>randomvariable!C6 *10</f>
@@ -1459,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,7 +1464,7 @@
         <v>0.2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>0</v>
@@ -1485,7 +1479,7 @@
         <v>-3.5000000000000004E-5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>19</v>
@@ -1500,25 +1494,10 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B38" s="1">
-        <f>5*10^(-5)</f>
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>